<commit_message>
+ SaveInvoice now updates source timesheet's Invoicing worksheet
To represent that a new invoice has been created.
</commit_message>
<xml_diff>
--- a/TestData/Invoicing/Invoice Seed.xlsx
+++ b/TestData/Invoicing/Invoice Seed.xlsx
@@ -12,10 +12,8 @@
   <definedNames>
     <definedName name="CustomerID">'Service Invoice'!$F$5</definedName>
     <definedName name="InvoiceNumber">'Service Invoice'!$F$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Service Invoice'!$A$1:$F$24</definedName>
-    <definedName name="TotalHoursWorked">'Service Invoice'!$D$19</definedName>
-    <definedName name="TotalPay">'Service Invoice'!$F$21</definedName>
-    <definedName name="Z_260B2C2D_8AED_4F5D_BB9A_A5CC9A317F2F_.wvu.PrintArea" localSheetId="0" hidden="1">'Service Invoice'!$A$1:$F$24</definedName>
+    <definedName name="TotalHoursWorked">'Service Invoice'!$D$16</definedName>
+    <definedName name="TotalPay">'Service Invoice'!$F$18</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
@@ -101,7 +99,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="[h]:mm"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -244,12 +242,6 @@
       <b/>
       <sz val="9"/>
       <color indexed="9"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="61"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -344,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -439,20 +431,8 @@
     <xf numFmtId="44" fontId="20" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="20" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,12 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="20" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -653,8 +627,23 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B1C07B7B-C3B9-4BDD-B3BA-A582EFA0CCB3}">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0B05CB80-D4C3-40AA-BD38-B09380DF401B}" diskRevisions="1" revisionId="6" version="4">
   <header guid="{B1C07B7B-C3B9-4BDD-B3BA-A582EFA0CCB3}" dateTime="2014-11-28T13:40:38" maxSheetId="2" userName="Paul" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{72D03F5D-88DA-41D7-B2A3-7B9047B42A8C}" dateTime="2014-11-29T16:46:29" maxSheetId="2" userName="Paul" r:id="rId2">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{69DEBFA0-38D6-4745-9ACE-7E4BE88F7A76}" dateTime="2014-11-29T18:34:27" maxSheetId="2" userName="Paul" r:id="rId3" minRId="2" maxRId="4">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0B05CB80-D4C3-40AA-BD38-B09380DF401B}" dateTime="2014-11-29T18:42:52" maxSheetId="2" userName="Paul" r:id="rId4">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -664,6 +653,607 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_260B2C2D_8AED_4F5D_BB9A_A5CC9A317F2F_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <formula>'Service Invoice'!$A$1:$F$24</formula>
+    <oldFormula>'Service Invoice'!$A$1:$F$24</oldFormula>
+  </rdn>
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="2" sId="1" ref="A15:XFD15" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A15:XFD15" start="0" length="0">
+      <dxf>
+        <font>
+          <name val="Palatino Linotype"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="A15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="C15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="166" formatCode="[h]:mm"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="35" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="40"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="3" sId="1" ref="A15:XFD15" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A15:XFD15" start="0" length="0"/>
+    <rfmt sheetId="1" sqref="A15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="9"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="9"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="C15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="9"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="9"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="166" formatCode="[h]:mm"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="9"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="E15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="9"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="F15" start="0" length="0">
+      <dxf>
+        <font>
+          <sz val="10"/>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="40"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+  </rrc>
+  <rrc rId="4" sId="1" ref="A15:XFD15" action="deleteRow">
+    <rfmt sheetId="1" xfDxf="1" sqref="A15:XFD15" start="0" length="0">
+      <dxf>
+        <font>
+          <name val="Palatino Linotype"/>
+          <scheme val="none"/>
+        </font>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="A15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="B15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="C15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rfmt sheetId="1" sqref="D15" start="0" length="0">
+      <dxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="166" formatCode="[h]:mm"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </dxf>
+    </rfmt>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="E15">
+        <f>IF(ISBLANK(D15),"",50)</f>
+      </nc>
+      <ndxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="46"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="1" dxf="1">
+      <nc r="F15">
+        <f>IF(D15&gt;0,D15*E15*24,"")</f>
+      </nc>
+      <ndxf>
+        <font>
+          <color indexed="61"/>
+          <name val="Tahoma"/>
+          <scheme val="none"/>
+        </font>
+        <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+        <fill>
+          <patternFill patternType="solid">
+            <bgColor indexed="40"/>
+          </patternFill>
+        </fill>
+        <alignment vertical="center" readingOrder="0"/>
+        <border outline="0">
+          <left style="thin">
+            <color indexed="41"/>
+          </left>
+          <right style="thin">
+            <color indexed="41"/>
+          </right>
+          <top style="thin">
+            <color indexed="41"/>
+          </top>
+          <bottom style="thin">
+            <color indexed="41"/>
+          </bottom>
+        </border>
+      </ndxf>
+    </rcc>
+  </rrc>
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_260B2C2D_8AED_4F5D_BB9A_A5CC9A317F2F_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <formula>'Service Invoice'!$A$1:$F$21</formula>
+    <oldFormula>'Service Invoice'!$A$1:$F$21</oldFormula>
+  </rdn>
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_260B2C2D_8AED_4F5D_BB9A_A5CC9A317F2F_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <oldFormula>'Service Invoice'!$A$1:$F$21</oldFormula>
+  </rdn>
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="delete"/>
+  <rcv guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -957,15 +1547,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" style="2" customWidth="1"/>
+    <col min="1" max="2" width="12.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.21875" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
@@ -974,13 +1563,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="58.5" customHeight="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A1" s="1"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -991,11 +1580,11 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22" t="s">
         <v>1</v>
@@ -1003,11 +1592,11 @@
       <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="24"/>
       <c r="E4" s="27" t="s">
         <v>6</v>
@@ -1015,11 +1604,11 @@
       <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="53"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="25"/>
       <c r="E5" s="27" t="s">
         <v>0</v>
@@ -1031,48 +1620,48 @@
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
-      <c r="E6" s="49"/>
+      <c r="E6" s="45"/>
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="1:6" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="65"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="46" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="28"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
       <c r="D8" s="26"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:6" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:6" s="7" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="22"/>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="46" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1081,8 +1670,8 @@
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
@@ -1102,7 +1691,7 @@
       <c r="C13" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="51" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="32" t="s">
@@ -1121,151 +1710,121 @@
       <c r="F14" s="39"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="39"/>
-    </row>
-    <row r="16" spans="1:6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="39" t="str">
+        <f t="shared" ref="F15" si="0">IF(D15&gt;0,D15*E15*24,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="40">
+        <f>SUM(D14:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="39" t="str">
+        <f>IF(SUM(F14:F15)&gt;0,SUM(F14:F15),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="40"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="43"/>
-      <c r="E17" s="56" t="str">
-        <f t="shared" ref="E17" si="0">IF(ISBLANK(D17),"",50)</f>
+      <c r="E17" s="44"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="43"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="39" t="str">
+        <f>IF(SUM(F16)&gt;0,SUM((F16*F17)+F16),"")</f>
         <v/>
       </c>
-      <c r="F17" s="39" t="str">
-        <f t="shared" ref="F17:F18" si="1">IF(D17&gt;0,D17*E17*24,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="39" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="46"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="43">
-        <f>SUM(D14:D18)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="48" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="39" t="str">
-        <f>IF(SUM(F14:F18)&gt;0,SUM(F14:F18),"")</f>
-        <v/>
-      </c>
+      <c r="A19" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="47"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="45"/>
+      <c r="A20" s="55" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="39" t="str">
-        <f>IF(SUM(F19)&gt;0,SUM((F19*F20)+F19),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="60" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="60"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-    </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="61" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-    </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="62"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-    </row>
-    <row r="25" spans="1:6" ht="9.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="58"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="18"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="20"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+    </row>
+    <row r="22" spans="1:6" ht="9.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="52"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="20"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" showGridLines="0">
+    <customSheetView guid="{260B2C2D-8AED-4F5D-BB9A-A5CC9A317F2F}" showPageBreaks="1" showGridLines="0">
       <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
       <printOptions horizontalCentered="1"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1273,9 +1832,9 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F24"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:F21"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="B7:C7"/>

</xml_diff>